<commit_message>
fix typo in tags
</commit_message>
<xml_diff>
--- a/automation/mrz_himmelheber/Meta_Himmelheber_Fotos.xlsx
+++ b/automation/mrz_himmelheber/Meta_Himmelheber_Fotos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sszsim\opendatazurich\opendatazurich.github.io\automation\mrz_himmelheber\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Python\git\opendatazurich.github.io\automation\mrz_himmelheber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06BA664-2331-4052-A6E8-E63AE818B9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB81F56-9FE0-4976-B2A7-675F6C2C4A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23688" yWindow="1500" windowWidth="21516" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5985" yWindow="5025" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -1111,10 +1111,10 @@
     <t>Fotos im Archiv von Hans Himmelheber (1908–2003) im Museum Rietberg</t>
   </si>
   <si>
-    <t>Fotografie, Archiv, Kunst, Ethnologie, Reisen, Himmelheber, Afirka, Alaska</t>
-  </si>
-  <si>
     <t>Museum Rietberg, Präsidialdepartement</t>
+  </si>
+  <si>
+    <t>Fotografie, Archiv, Kunst, Ethnologie, Reisen, Himmelheber, Afrika, Alaska</t>
   </si>
 </sst>
 </file>
@@ -1855,22 +1855,22 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" style="11" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="66.83203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="53.58203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="66.875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.625" style="5" customWidth="1"/>
     <col min="5" max="5" width="8.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="88.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>31</v>
       </c>
@@ -1992,14 +1992,14 @@
         <v>14</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -2010,14 +2010,14 @@
         <v>14</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>33</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>49</v>
       </c>
@@ -2134,14 +2134,14 @@
         <v>14</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>52</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
         <v>130</v>
       </c>
@@ -2177,14 +2177,14 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
@@ -2197,7 +2197,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
@@ -2207,7 +2207,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="137.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="62.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
@@ -2237,7 +2237,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" ht="43" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>51</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>51</v>
       </c>
@@ -2268,31 +2268,31 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="24"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D26" s="24"/>
       <c r="E26" s="7"/>
       <c r="F26" s="24"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="1"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="1"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2300,7 +2300,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="13" t="s">
         <v>26</v>
@@ -2334,7 +2334,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="62.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>30</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="62.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>30</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>30</v>
       </c>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>30</v>
       </c>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="4" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>30</v>
       </c>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:6" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>30</v>
       </c>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>30</v>
       </c>
@@ -2508,7 +2508,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>30</v>
       </c>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>30</v>
       </c>
@@ -2547,7 +2547,7 @@
       <c r="D45" s="22"/>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>30</v>
       </c>
@@ -2556,28 +2556,28 @@
       <c r="D46" s="22"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="11"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
       <c r="B50" s="3" t="s">
         <v>161</v>
@@ -2586,14 +2586,14 @@
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>157</v>
       </c>
@@ -2607,7 +2607,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B53" s="13" t="s">
         <v>158</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -2641,131 +2641,131 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.58203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.58203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.58203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" style="25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.75" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.58203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.875" style="25" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="34" t="s">
         <v>129</v>
       </c>
@@ -2787,14 +2787,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="5.58203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="25" customWidth="1"/>
     <col min="3" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>71</v>
       </c>
@@ -2802,27 +2802,27 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>72</v>
       </c>
@@ -2830,12 +2830,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
         <v>129</v>
       </c>
@@ -2857,14 +2857,14 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.25" style="25" customWidth="1"/>
     <col min="3" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>71</v>
       </c>
@@ -2872,118 +2872,118 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
     </row>
-    <row r="19" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
     </row>
-    <row r="23" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
     </row>
-    <row r="24" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
     </row>
-    <row r="25" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
     </row>
-    <row r="26" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
     </row>
-    <row r="27" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
     </row>
   </sheetData>
@@ -3003,15 +3003,15 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="58.58203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="58.625" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>71</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>88</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>89</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>90</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>91</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>92</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
         <v>93</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>94</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>95</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>96</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>97</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>98</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>99</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>100</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>101</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
         <v>102</v>
       </c>
@@ -3202,12 +3202,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
         <v>129</v>
       </c>
@@ -3224,21 +3224,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3352,17 +3337,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3376,17 +3377,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>